<commit_message>
Finale Version Word Zeitplanung bis zum 13.12
</commit_message>
<xml_diff>
--- a/Zeitplanung Marvin Purtschert.xlsx
+++ b/Zeitplanung Marvin Purtschert.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="DieseArbeitsmappe" showPivotChartFilter="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://calida365-my.sharepoint.com/personal/marvin_purtschert_calida_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BLJ\LED-Connection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{482CA84E-9558-407F-B9A4-1487CC2EC787}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{50173739-935E-497D-BBE6-E7CD8B2756B9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D6B356-5B64-4894-98A2-B9282C841B84}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="55">
   <si>
     <t>Nr.</t>
   </si>
@@ -125,9 +125,6 @@
     <t>Ist</t>
   </si>
   <si>
-    <t>&lt;Projektname&gt;</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -152,9 +149,6 @@
     <t>Anforderung #01</t>
   </si>
   <si>
-    <t>Anforderung #02</t>
-  </si>
-  <si>
     <t>Anforderung #03</t>
   </si>
   <si>
@@ -165,15 +159,6 @@
   </si>
   <si>
     <t>Anforderung #06</t>
-  </si>
-  <si>
-    <t>Anforderung #07</t>
-  </si>
-  <si>
-    <t>Anforderung #08</t>
-  </si>
-  <si>
-    <t>Anforderung #09</t>
   </si>
   <si>
     <t>Testfälle erstellen</t>
@@ -189,9 +174,6 @@
   </si>
   <si>
     <t>Anforderungsanalyse  (Was)</t>
-  </si>
-  <si>
-    <t>Lösungsvarianten ausarbeiten (Wie)</t>
   </si>
   <si>
     <t xml:space="preserve"> Abwesend (Ferien/Schule)</t>
@@ -255,6 +237,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>&lt;LED-Connection&gt;</t>
   </si>
 </sst>
 </file>
@@ -1403,6 +1388,10 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1433,10 +1422,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1541,7 +1526,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>69</c:v>
@@ -1553,7 +1538,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1612,13 +1597,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2125,8 +2110,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="BK25" sqref="BK25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2142,7 +2127,7 @@
   <sheetData>
     <row r="1" spans="1:62" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2247,7 +2232,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="86"/>
       <c r="H3" s="23" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
@@ -2377,7 +2362,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="22"/>
       <c r="H5" s="23" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="I5" s="23"/>
       <c r="J5" s="6"/>
@@ -2445,88 +2430,88 @@
     <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="27"/>
-      <c r="C7" s="90" t="s">
+      <c r="C7" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="90"/>
+      <c r="D7" s="91"/>
       <c r="E7" s="28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="91" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="92" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="92"/>
+      <c r="I7" s="92"/>
+      <c r="J7" s="92"/>
+      <c r="K7" s="92"/>
+      <c r="L7" s="92"/>
+      <c r="M7" s="93"/>
+      <c r="N7" s="92" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7" s="92"/>
+      <c r="P7" s="92"/>
+      <c r="Q7" s="92"/>
+      <c r="R7" s="92"/>
+      <c r="S7" s="92"/>
+      <c r="T7" s="93"/>
+      <c r="U7" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="V7" s="92"/>
+      <c r="W7" s="92"/>
+      <c r="X7" s="92"/>
+      <c r="Y7" s="92"/>
+      <c r="Z7" s="92"/>
+      <c r="AA7" s="93"/>
+      <c r="AB7" s="94" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC7" s="92"/>
+      <c r="AD7" s="92"/>
+      <c r="AE7" s="92"/>
+      <c r="AF7" s="92"/>
+      <c r="AG7" s="92"/>
+      <c r="AH7" s="93"/>
+      <c r="AI7" s="92" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ7" s="92"/>
+      <c r="AK7" s="92"/>
+      <c r="AL7" s="92"/>
+      <c r="AM7" s="92"/>
+      <c r="AN7" s="92"/>
+      <c r="AO7" s="93"/>
+      <c r="AP7" s="94" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ7" s="92"/>
+      <c r="AR7" s="92"/>
+      <c r="AS7" s="92"/>
+      <c r="AT7" s="92"/>
+      <c r="AU7" s="92"/>
+      <c r="AV7" s="93"/>
+      <c r="AW7" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="91"/>
-      <c r="I7" s="91"/>
-      <c r="J7" s="91"/>
-      <c r="K7" s="91"/>
-      <c r="L7" s="91"/>
-      <c r="M7" s="92"/>
-      <c r="N7" s="91" t="s">
+      <c r="AX7" s="92"/>
+      <c r="AY7" s="92"/>
+      <c r="AZ7" s="92"/>
+      <c r="BA7" s="92"/>
+      <c r="BB7" s="92"/>
+      <c r="BC7" s="93"/>
+      <c r="BD7" s="94" t="s">
         <v>46</v>
       </c>
-      <c r="O7" s="91"/>
-      <c r="P7" s="91"/>
-      <c r="Q7" s="91"/>
-      <c r="R7" s="91"/>
-      <c r="S7" s="91"/>
-      <c r="T7" s="92"/>
-      <c r="U7" s="91" t="s">
-        <v>47</v>
-      </c>
-      <c r="V7" s="91"/>
-      <c r="W7" s="91"/>
-      <c r="X7" s="91"/>
-      <c r="Y7" s="91"/>
-      <c r="Z7" s="91"/>
-      <c r="AA7" s="92"/>
-      <c r="AB7" s="93" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC7" s="91"/>
-      <c r="AD7" s="91"/>
-      <c r="AE7" s="91"/>
-      <c r="AF7" s="91"/>
-      <c r="AG7" s="91"/>
-      <c r="AH7" s="92"/>
-      <c r="AI7" s="91" t="s">
-        <v>49</v>
-      </c>
-      <c r="AJ7" s="91"/>
-      <c r="AK7" s="91"/>
-      <c r="AL7" s="91"/>
-      <c r="AM7" s="91"/>
-      <c r="AN7" s="91"/>
-      <c r="AO7" s="92"/>
-      <c r="AP7" s="93" t="s">
-        <v>50</v>
-      </c>
-      <c r="AQ7" s="91"/>
-      <c r="AR7" s="91"/>
-      <c r="AS7" s="91"/>
-      <c r="AT7" s="91"/>
-      <c r="AU7" s="91"/>
-      <c r="AV7" s="92"/>
-      <c r="AW7" s="91" t="s">
-        <v>51</v>
-      </c>
-      <c r="AX7" s="91"/>
-      <c r="AY7" s="91"/>
-      <c r="AZ7" s="91"/>
-      <c r="BA7" s="91"/>
-      <c r="BB7" s="91"/>
-      <c r="BC7" s="92"/>
-      <c r="BD7" s="93" t="s">
-        <v>52</v>
-      </c>
-      <c r="BE7" s="91"/>
-      <c r="BF7" s="91"/>
-      <c r="BG7" s="91"/>
-      <c r="BH7" s="91"/>
-      <c r="BI7" s="91"/>
-      <c r="BJ7" s="94"/>
+      <c r="BE7" s="92"/>
+      <c r="BF7" s="92"/>
+      <c r="BG7" s="92"/>
+      <c r="BH7" s="92"/>
+      <c r="BI7" s="92"/>
+      <c r="BJ7" s="95"/>
     </row>
     <row r="8" spans="1:62" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
@@ -2543,175 +2528,175 @@
         <v>4</v>
       </c>
       <c r="F8" s="34" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="I8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="L8" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="O8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="P8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="R8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="S8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="L8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="M8" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" s="14" t="s">
+      <c r="T8" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="U8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="V8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="O8" s="15" t="s">
+      <c r="W8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="X8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="P8" s="15" t="s">
+      <c r="Z8" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA8" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="Q8" s="14" t="s">
+      <c r="AD8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="R8" s="14" t="s">
+      <c r="AG8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="S8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="T8" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="U8" s="14" t="s">
+      <c r="AH8" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="V8" s="15" t="s">
+      <c r="AK8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="W8" s="15" t="s">
+      <c r="AN8" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO8" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AQ8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="X8" s="14" t="s">
+      <c r="AR8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="AS8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="AT8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="Y8" s="14" t="s">
+      <c r="AU8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="Z8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA8" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB8" s="16" t="s">
+      <c r="AV8" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="AW8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AX8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="AC8" s="15" t="s">
+      <c r="AY8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="BA8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="AD8" s="15" t="s">
+      <c r="BB8" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="BC8" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="BD8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="BE8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="AE8" s="14" t="s">
+      <c r="BF8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="BG8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="BH8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="AF8" s="14" t="s">
+      <c r="BI8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="AG8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="AH8" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="AI8" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="AJ8" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="AK8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="AL8" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="AM8" s="14" t="s">
+      <c r="BJ8" s="25" t="s">
         <v>19</v>
-      </c>
-      <c r="AN8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="AO8" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="AP8" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="AQ8" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="AR8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="AS8" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="AT8" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="AU8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="AV8" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="AW8" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="AX8" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="AY8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="AZ8" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="BA8" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="BB8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="BC8" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="BD8" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="BE8" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="BF8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="BG8" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="BH8" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="BI8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="BJ8" s="25" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2719,7 +2704,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="41">
         <f>SUM(C10:C13)</f>
@@ -2727,7 +2712,7 @@
       </c>
       <c r="D9" s="42">
         <f>SUM(D10:D13)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="31"/>
@@ -2796,14 +2781,14 @@
         <v>12</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D10" s="84"/>
       <c r="E10" s="48">
         <v>1</v>
       </c>
       <c r="F10" s="88" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G10" s="53"/>
       <c r="H10" s="54"/>
@@ -2814,7 +2799,7 @@
       <c r="M10" s="58"/>
       <c r="N10" s="53"/>
       <c r="O10" s="54"/>
-      <c r="P10" s="55"/>
+      <c r="P10" s="59"/>
       <c r="Q10" s="55"/>
       <c r="R10" s="56"/>
       <c r="S10" s="57"/>
@@ -2867,12 +2852,14 @@
         <v>102</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="49"/>
+        <v>37</v>
+      </c>
+      <c r="C11" s="49">
+        <v>2</v>
+      </c>
       <c r="D11" s="83">
         <f>SUM(G11:BJ11)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E11" s="50">
         <v>1</v>
@@ -2882,15 +2869,19 @@
       <c r="H11" s="60"/>
       <c r="I11" s="61"/>
       <c r="J11" s="61"/>
-      <c r="K11" s="85"/>
+      <c r="K11" s="85">
+        <v>2</v>
+      </c>
       <c r="L11" s="62"/>
       <c r="M11" s="58" t="s">
         <v>5</v>
       </c>
       <c r="N11" s="59"/>
       <c r="O11" s="60"/>
-      <c r="P11" s="61"/>
-      <c r="Q11" s="61"/>
+      <c r="P11" s="59"/>
+      <c r="Q11" s="61">
+        <v>1</v>
+      </c>
       <c r="R11" s="56"/>
       <c r="S11" s="57"/>
       <c r="T11" s="58" t="s">
@@ -2944,14 +2935,14 @@
         <v>103</v>
       </c>
       <c r="B12" s="45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="49">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D12" s="83">
         <f>SUM(G12:BJ12)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12" s="50">
         <v>1</v>
@@ -2961,14 +2952,18 @@
       <c r="H12" s="60"/>
       <c r="I12" s="61"/>
       <c r="J12" s="61"/>
-      <c r="K12" s="63"/>
+      <c r="K12" s="63">
+        <v>1</v>
+      </c>
       <c r="L12" s="57"/>
       <c r="M12" s="58"/>
       <c r="N12" s="59"/>
       <c r="O12" s="60"/>
-      <c r="P12" s="61"/>
+      <c r="P12" s="59"/>
       <c r="Q12" s="61"/>
-      <c r="R12" s="63"/>
+      <c r="R12" s="63">
+        <v>1</v>
+      </c>
       <c r="S12" s="57"/>
       <c r="T12" s="58"/>
       <c r="U12" s="59"/>
@@ -3019,17 +3014,17 @@
         <v>104</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D13" s="83"/>
       <c r="E13" s="50">
         <v>1</v>
       </c>
       <c r="F13" s="88" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G13" s="59"/>
       <c r="H13" s="60"/>
@@ -3040,7 +3035,7 @@
       <c r="M13" s="65"/>
       <c r="N13" s="59"/>
       <c r="O13" s="60"/>
-      <c r="P13" s="55"/>
+      <c r="P13" s="59"/>
       <c r="Q13" s="55"/>
       <c r="R13" s="55"/>
       <c r="S13" s="66"/>
@@ -3069,8 +3064,8 @@
       <c r="AP13" s="59"/>
       <c r="AQ13" s="60"/>
       <c r="AR13" s="55"/>
-      <c r="AS13" s="87"/>
-      <c r="AT13" s="55"/>
+      <c r="AS13" s="61"/>
+      <c r="AT13" s="87"/>
       <c r="AU13" s="66"/>
       <c r="AV13" s="67"/>
       <c r="AW13" s="59"/>
@@ -3097,11 +3092,11 @@
       </c>
       <c r="C14" s="41">
         <f>SUM(C15:C17)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D14" s="42">
         <f>SUM(D15:D17)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="31"/>
@@ -3167,27 +3162,33 @@
         <v>201</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="49"/>
+        <v>32</v>
+      </c>
+      <c r="C15" s="49">
+        <v>5</v>
+      </c>
       <c r="D15" s="83">
         <f>SUM(G15:BJ15)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E15" s="50"/>
       <c r="F15" s="89" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G15" s="53"/>
       <c r="H15" s="54"/>
-      <c r="I15" s="68"/>
-      <c r="J15" s="87"/>
-      <c r="K15" s="63"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="87">
+        <v>5</v>
+      </c>
+      <c r="K15" s="63">
+        <v>3</v>
+      </c>
       <c r="L15" s="57"/>
       <c r="M15" s="58"/>
       <c r="N15" s="53"/>
       <c r="O15" s="54"/>
-      <c r="P15" s="55"/>
+      <c r="P15" s="53"/>
       <c r="Q15" s="55"/>
       <c r="R15" s="56"/>
       <c r="S15" s="57"/>
@@ -3239,9 +3240,7 @@
       <c r="A16" s="12">
         <v>202</v>
       </c>
-      <c r="B16" s="46" t="s">
-        <v>38</v>
-      </c>
+      <c r="B16" s="46"/>
       <c r="C16" s="49"/>
       <c r="D16" s="83">
         <f>SUM(G16:BJ16)</f>
@@ -3258,7 +3257,7 @@
       <c r="M16" s="58"/>
       <c r="N16" s="59"/>
       <c r="O16" s="60"/>
-      <c r="P16" s="55"/>
+      <c r="P16" s="53"/>
       <c r="Q16" s="55"/>
       <c r="R16" s="56"/>
       <c r="S16" s="57"/>
@@ -3327,7 +3326,7 @@
       <c r="M17" s="58"/>
       <c r="N17" s="69"/>
       <c r="O17" s="70"/>
-      <c r="P17" s="55"/>
+      <c r="P17" s="53"/>
       <c r="Q17" s="55"/>
       <c r="R17" s="56"/>
       <c r="S17" s="57"/>
@@ -3388,7 +3387,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3454,7 +3453,7 @@
         <v>301</v>
       </c>
       <c r="B19" s="46" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C19" s="49"/>
       <c r="D19" s="83">
@@ -3472,7 +3471,7 @@
       <c r="M19" s="58"/>
       <c r="N19" s="53"/>
       <c r="O19" s="54"/>
-      <c r="P19" s="55"/>
+      <c r="P19" s="60"/>
       <c r="Q19" s="55"/>
       <c r="R19" s="56"/>
       <c r="S19" s="57"/>
@@ -3525,29 +3524,37 @@
         <v>302</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C20" s="49">
         <v>18</v>
       </c>
       <c r="D20" s="83">
         <f t="shared" ref="D20:D30" si="0">SUM(G20:BJ20)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E20" s="50"/>
       <c r="F20" s="51"/>
       <c r="G20" s="59"/>
       <c r="H20" s="60"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="68"/>
-      <c r="K20" s="63"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="68">
+        <v>3</v>
+      </c>
+      <c r="K20" s="63">
+        <v>1</v>
+      </c>
       <c r="L20" s="57"/>
       <c r="M20" s="58"/>
       <c r="N20" s="59"/>
       <c r="O20" s="60"/>
-      <c r="P20" s="55"/>
-      <c r="Q20" s="55"/>
-      <c r="R20" s="56"/>
+      <c r="P20" s="60"/>
+      <c r="Q20" s="68">
+        <v>2</v>
+      </c>
+      <c r="R20" s="56">
+        <v>4</v>
+      </c>
       <c r="S20" s="57"/>
       <c r="T20" s="58"/>
       <c r="U20" s="59"/>
@@ -3598,19 +3605,21 @@
         <v>303</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="49">
         <v>24</v>
       </c>
       <c r="D21" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E21" s="50">
         <v>1</v>
       </c>
-      <c r="F21" s="52"/>
+      <c r="F21" s="52">
+        <v>19.12</v>
+      </c>
       <c r="G21" s="59"/>
       <c r="H21" s="60"/>
       <c r="I21" s="55"/>
@@ -3620,15 +3629,19 @@
       <c r="M21" s="58"/>
       <c r="N21" s="59"/>
       <c r="O21" s="60"/>
-      <c r="P21" s="68"/>
-      <c r="Q21" s="68"/>
-      <c r="R21" s="63"/>
+      <c r="P21" s="60"/>
+      <c r="Q21" s="68">
+        <v>5</v>
+      </c>
+      <c r="R21" s="63">
+        <v>2</v>
+      </c>
       <c r="S21" s="57"/>
       <c r="T21" s="58"/>
       <c r="U21" s="59"/>
       <c r="V21" s="60"/>
       <c r="W21" s="68"/>
-      <c r="X21" s="55"/>
+      <c r="X21" s="87"/>
       <c r="Y21" s="56"/>
       <c r="Z21" s="57"/>
       <c r="AA21" s="58"/>
@@ -3668,13 +3681,11 @@
       <c r="BI21" s="57"/>
       <c r="BJ21" s="58"/>
     </row>
-    <row r="22" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:62" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>304</v>
       </c>
-      <c r="B22" s="46" t="s">
-        <v>25</v>
-      </c>
+      <c r="B22" s="46"/>
       <c r="C22" s="49"/>
       <c r="D22" s="83">
         <f t="shared" si="0"/>
@@ -3693,7 +3704,7 @@
       <c r="M22" s="58"/>
       <c r="N22" s="59"/>
       <c r="O22" s="60"/>
-      <c r="P22" s="55"/>
+      <c r="P22" s="60"/>
       <c r="Q22" s="55"/>
       <c r="R22" s="56"/>
       <c r="S22" s="57"/>
@@ -3746,7 +3757,7 @@
         <v>305</v>
       </c>
       <c r="B23" s="46" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C23" s="49">
         <v>6</v>
@@ -3761,14 +3772,14 @@
       <c r="F23" s="51"/>
       <c r="G23" s="59"/>
       <c r="H23" s="60"/>
-      <c r="I23" s="61"/>
+      <c r="I23" s="55"/>
       <c r="J23" s="61"/>
       <c r="K23" s="56"/>
       <c r="L23" s="57"/>
       <c r="M23" s="58"/>
       <c r="N23" s="59"/>
       <c r="O23" s="60"/>
-      <c r="P23" s="61"/>
+      <c r="P23" s="60"/>
       <c r="Q23" s="61"/>
       <c r="R23" s="56"/>
       <c r="S23" s="57"/>
@@ -3776,8 +3787,8 @@
       <c r="U23" s="59"/>
       <c r="V23" s="60"/>
       <c r="W23" s="61"/>
-      <c r="X23" s="99"/>
-      <c r="Y23" s="56"/>
+      <c r="X23" s="61"/>
+      <c r="Y23" s="90"/>
       <c r="Z23" s="57"/>
       <c r="AA23" s="58"/>
       <c r="AB23" s="59"/>
@@ -3796,7 +3807,7 @@
       <c r="AO23" s="58"/>
       <c r="AP23" s="59"/>
       <c r="AQ23" s="60"/>
-      <c r="AR23" s="61"/>
+      <c r="AR23" s="90"/>
       <c r="AS23" s="61"/>
       <c r="AT23" s="56"/>
       <c r="AU23" s="57"/>
@@ -3821,14 +3832,14 @@
         <v>306</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C24" s="49">
         <v>15</v>
       </c>
       <c r="D24" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="50">
         <v>1</v>
@@ -3836,16 +3847,18 @@
       <c r="F24" s="51"/>
       <c r="G24" s="59"/>
       <c r="H24" s="60"/>
-      <c r="I24" s="68"/>
+      <c r="I24" s="55"/>
       <c r="J24" s="68"/>
       <c r="K24" s="63"/>
       <c r="L24" s="57"/>
       <c r="M24" s="58"/>
       <c r="N24" s="59"/>
       <c r="O24" s="60"/>
-      <c r="P24" s="68"/>
+      <c r="P24" s="60"/>
       <c r="Q24" s="68"/>
-      <c r="R24" s="63"/>
+      <c r="R24" s="63">
+        <v>1</v>
+      </c>
       <c r="S24" s="57"/>
       <c r="T24" s="58"/>
       <c r="U24" s="59"/>
@@ -3896,7 +3909,7 @@
         <v>307</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C25" s="49">
         <v>6</v>
@@ -3918,7 +3931,7 @@
       <c r="M25" s="58"/>
       <c r="N25" s="59"/>
       <c r="O25" s="60"/>
-      <c r="P25" s="55"/>
+      <c r="P25" s="60"/>
       <c r="Q25" s="55"/>
       <c r="R25" s="56"/>
       <c r="S25" s="57"/>
@@ -3927,7 +3940,7 @@
       <c r="V25" s="60"/>
       <c r="W25" s="55"/>
       <c r="X25" s="55"/>
-      <c r="Y25" s="63"/>
+      <c r="Y25" s="55"/>
       <c r="Z25" s="57"/>
       <c r="AA25" s="58"/>
       <c r="AB25" s="59"/>
@@ -3947,8 +3960,8 @@
       <c r="AP25" s="59"/>
       <c r="AQ25" s="60"/>
       <c r="AR25" s="55"/>
-      <c r="AS25" s="55"/>
-      <c r="AT25" s="56"/>
+      <c r="AS25" s="68"/>
+      <c r="AT25" s="68"/>
       <c r="AU25" s="57"/>
       <c r="AV25" s="58"/>
       <c r="AW25" s="59"/>
@@ -3971,7 +3984,7 @@
         <v>308</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C26" s="49"/>
       <c r="D26" s="83">
@@ -3991,7 +4004,7 @@
       <c r="M26" s="58"/>
       <c r="N26" s="59"/>
       <c r="O26" s="60"/>
-      <c r="P26" s="55"/>
+      <c r="P26" s="60"/>
       <c r="Q26" s="55"/>
       <c r="R26" s="56"/>
       <c r="S26" s="57"/>
@@ -4043,9 +4056,7 @@
       <c r="A27" s="12">
         <v>309</v>
       </c>
-      <c r="B27" s="46" t="s">
-        <v>30</v>
-      </c>
+      <c r="B27" s="46"/>
       <c r="C27" s="49"/>
       <c r="D27" s="83">
         <f t="shared" si="0"/>
@@ -4062,7 +4073,7 @@
       <c r="M27" s="58"/>
       <c r="N27" s="59"/>
       <c r="O27" s="60"/>
-      <c r="P27" s="55"/>
+      <c r="P27" s="60"/>
       <c r="Q27" s="55"/>
       <c r="R27" s="56"/>
       <c r="S27" s="57"/>
@@ -4114,9 +4125,7 @@
       <c r="A28" s="12">
         <v>310</v>
       </c>
-      <c r="B28" s="46" t="s">
-        <v>31</v>
-      </c>
+      <c r="B28" s="46"/>
       <c r="C28" s="49"/>
       <c r="D28" s="83">
         <f t="shared" si="0"/>
@@ -4133,7 +4142,7 @@
       <c r="M28" s="58"/>
       <c r="N28" s="59"/>
       <c r="O28" s="60"/>
-      <c r="P28" s="55"/>
+      <c r="P28" s="60"/>
       <c r="Q28" s="55"/>
       <c r="R28" s="56"/>
       <c r="S28" s="57"/>
@@ -4185,9 +4194,7 @@
       <c r="A29" s="12">
         <v>311</v>
       </c>
-      <c r="B29" s="46" t="s">
-        <v>32</v>
-      </c>
+      <c r="B29" s="46"/>
       <c r="C29" s="49"/>
       <c r="D29" s="83">
         <f t="shared" si="0"/>
@@ -4204,7 +4211,7 @@
       <c r="M29" s="58"/>
       <c r="N29" s="71"/>
       <c r="O29" s="72"/>
-      <c r="P29" s="55"/>
+      <c r="P29" s="60"/>
       <c r="Q29" s="55"/>
       <c r="R29" s="56"/>
       <c r="S29" s="57"/>
@@ -4273,7 +4280,7 @@
       <c r="M30" s="58"/>
       <c r="N30" s="69"/>
       <c r="O30" s="70"/>
-      <c r="P30" s="55"/>
+      <c r="P30" s="60"/>
       <c r="Q30" s="55"/>
       <c r="R30" s="56"/>
       <c r="S30" s="57"/>
@@ -4400,7 +4407,7 @@
         <v>401</v>
       </c>
       <c r="B32" s="46" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C32" s="49"/>
       <c r="D32" s="83">
@@ -4418,7 +4425,7 @@
       <c r="M32" s="58"/>
       <c r="N32" s="53"/>
       <c r="O32" s="54"/>
-      <c r="P32" s="55"/>
+      <c r="P32" s="69"/>
       <c r="Q32" s="55"/>
       <c r="R32" s="56"/>
       <c r="S32" s="57"/>
@@ -4471,7 +4478,7 @@
         <v>402</v>
       </c>
       <c r="B33" s="46" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C33" s="49"/>
       <c r="D33" s="83">
@@ -4489,7 +4496,7 @@
       <c r="M33" s="58"/>
       <c r="N33" s="59"/>
       <c r="O33" s="60"/>
-      <c r="P33" s="55"/>
+      <c r="P33" s="69"/>
       <c r="Q33" s="55"/>
       <c r="R33" s="56"/>
       <c r="S33" s="57"/>
@@ -4542,7 +4549,7 @@
         <v>403</v>
       </c>
       <c r="B34" s="46" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C34" s="49"/>
       <c r="D34" s="83">
@@ -4560,7 +4567,7 @@
       <c r="M34" s="58"/>
       <c r="N34" s="59"/>
       <c r="O34" s="60"/>
-      <c r="P34" s="55"/>
+      <c r="P34" s="69"/>
       <c r="Q34" s="55"/>
       <c r="R34" s="56"/>
       <c r="S34" s="57"/>
@@ -4629,7 +4636,7 @@
       <c r="M35" s="58"/>
       <c r="N35" s="69"/>
       <c r="O35" s="70"/>
-      <c r="P35" s="55"/>
+      <c r="P35" s="69"/>
       <c r="Q35" s="55"/>
       <c r="R35" s="56"/>
       <c r="S35" s="57"/>
@@ -4756,7 +4763,7 @@
         <v>501</v>
       </c>
       <c r="B37" s="46" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C37" s="49"/>
       <c r="D37" s="83">
@@ -4774,7 +4781,7 @@
       <c r="M37" s="58"/>
       <c r="N37" s="53"/>
       <c r="O37" s="54"/>
-      <c r="P37" s="55"/>
+      <c r="P37" s="60"/>
       <c r="Q37" s="55"/>
       <c r="R37" s="56"/>
       <c r="S37" s="57"/>
@@ -4843,7 +4850,7 @@
       <c r="M38" s="58"/>
       <c r="N38" s="69"/>
       <c r="O38" s="70"/>
-      <c r="P38" s="55"/>
+      <c r="P38" s="60"/>
       <c r="Q38" s="55"/>
       <c r="R38" s="56"/>
       <c r="S38" s="57"/>
@@ -4900,7 +4907,7 @@
       </c>
       <c r="C39" s="41">
         <f>SUM(C40:C42)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D39" s="42">
         <f>SUM(D40:D42)</f>
@@ -4970,9 +4977,11 @@
         <v>601</v>
       </c>
       <c r="B40" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" s="49"/>
+        <v>34</v>
+      </c>
+      <c r="C40" s="49">
+        <v>2</v>
+      </c>
       <c r="D40" s="83">
         <f>SUM(G40:BJ40)</f>
         <v>0</v>
@@ -4988,7 +4997,7 @@
       <c r="M40" s="58"/>
       <c r="N40" s="53"/>
       <c r="O40" s="54"/>
-      <c r="P40" s="55"/>
+      <c r="P40" s="69"/>
       <c r="Q40" s="55"/>
       <c r="R40" s="56"/>
       <c r="S40" s="57"/>
@@ -5018,7 +5027,7 @@
       <c r="AQ40" s="54"/>
       <c r="AR40" s="55"/>
       <c r="AS40" s="55"/>
-      <c r="AT40" s="56"/>
+      <c r="AT40" s="68"/>
       <c r="AU40" s="57"/>
       <c r="AV40" s="58"/>
       <c r="AW40" s="53"/>
@@ -5041,9 +5050,11 @@
         <v>602</v>
       </c>
       <c r="B41" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="C41" s="49"/>
+        <v>35</v>
+      </c>
+      <c r="C41" s="49">
+        <v>1</v>
+      </c>
       <c r="D41" s="83">
         <f t="shared" ref="D41:D42" si="2">SUM(G41:BJ41)</f>
         <v>0</v>
@@ -5059,7 +5070,7 @@
       <c r="M41" s="58"/>
       <c r="N41" s="59"/>
       <c r="O41" s="60"/>
-      <c r="P41" s="55"/>
+      <c r="P41" s="69"/>
       <c r="Q41" s="55"/>
       <c r="R41" s="56"/>
       <c r="S41" s="57"/>
@@ -5089,7 +5100,7 @@
       <c r="AQ41" s="60"/>
       <c r="AR41" s="55"/>
       <c r="AS41" s="55"/>
-      <c r="AT41" s="56"/>
+      <c r="AT41" s="90"/>
       <c r="AU41" s="57"/>
       <c r="AV41" s="58"/>
       <c r="AW41" s="59"/>
@@ -5128,7 +5139,7 @@
       <c r="M42" s="58"/>
       <c r="N42" s="69"/>
       <c r="O42" s="70"/>
-      <c r="P42" s="55"/>
+      <c r="P42" s="69"/>
       <c r="Q42" s="55"/>
       <c r="R42" s="56"/>
       <c r="S42" s="57"/>
@@ -5183,11 +5194,11 @@
       </c>
       <c r="C43" s="37">
         <f>C39+C36+C31+C18+C14+C9</f>
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5205,11 +5216,11 @@
       </c>
       <c r="J43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L43" s="39">
         <f t="shared" si="3"/>
@@ -5233,11 +5244,11 @@
       </c>
       <c r="Q43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S43" s="39">
         <f t="shared" si="3"/>
@@ -5417,7 +5428,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" scenarios="1" formatCells="0"/>
+  <sheetProtection formatCells="0"/>
   <mergeCells count="9">
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="G7:M7"/>
@@ -5462,10 +5473,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="98"/>
+      <c r="B2" s="99"/>
       <c r="C2" s="79" t="s">
         <v>14</v>
       </c>
@@ -5474,62 +5485,62 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="95" t="str">
+      <c r="A3" s="96" t="str">
         <f>Zeitplanung!B9</f>
         <v>Administration, Planung</v>
       </c>
-      <c r="B3" s="96"/>
+      <c r="B3" s="97"/>
       <c r="C3" s="80">
         <f>Zeitplanung!C9</f>
         <v>5</v>
       </c>
       <c r="D3" s="80">
         <f>Zeitplanung!D9</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E3" s="82"/>
       <c r="F3" s="81"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="95" t="str">
+      <c r="A4" s="96" t="str">
         <f>Zeitplanung!B14</f>
         <v>Analyse &amp; Design</v>
       </c>
-      <c r="B4" s="96"/>
+      <c r="B4" s="97"/>
       <c r="C4" s="80">
         <f>Zeitplanung!C14</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D4" s="80">
         <f>Zeitplanung!D14</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E4" s="82"/>
       <c r="F4" s="81"/>
     </row>
     <row r="5" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="95" t="str">
+      <c r="A5" s="96" t="str">
         <f>Zeitplanung!B18</f>
         <v>Implementation</v>
       </c>
-      <c r="B5" s="96"/>
+      <c r="B5" s="97"/>
       <c r="C5" s="80">
         <f>Zeitplanung!C18</f>
         <v>69</v>
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>
     </row>
     <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="95" t="str">
+      <c r="A6" s="96" t="str">
         <f>Zeitplanung!B31</f>
         <v>Testen</v>
       </c>
-      <c r="B6" s="96"/>
+      <c r="B6" s="97"/>
       <c r="C6" s="80">
         <f>Zeitplanung!C31</f>
         <v>0</v>
@@ -5541,11 +5552,11 @@
       <c r="F6" s="81"/>
     </row>
     <row r="7" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="95" t="str">
+      <c r="A7" s="96" t="str">
         <f>Zeitplanung!B36</f>
         <v>Diverses</v>
       </c>
-      <c r="B7" s="96"/>
+      <c r="B7" s="97"/>
       <c r="C7" s="80">
         <f>Zeitplanung!C36</f>
         <v>0</v>
@@ -5557,14 +5568,14 @@
       <c r="F7" s="81"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="95" t="str">
+      <c r="A8" s="96" t="str">
         <f>Zeitplanung!B39</f>
         <v>Abschluss</v>
       </c>
-      <c r="B8" s="96"/>
+      <c r="B8" s="97"/>
       <c r="C8" s="80">
         <f>Zeitplanung!C39</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D8" s="80">
         <f>Zeitplanung!D39</f>
@@ -5590,6 +5601,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000BE50D1F786772468C3BF4B005DEE27E" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="514fbc13ac210c47c8dfd86ded7b5e79">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="747d6e8b-402a-417f-9569-0d05ef823c15" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f0f480f271c99990689b655dc5df90c3" ns3:_="">
     <xsd:import namespace="747d6e8b-402a-417f-9569-0d05ef823c15"/>
@@ -5721,22 +5747,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{915DD9A7-7D8D-4B51-8AB7-8EA01404FD44}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="747d6e8b-402a-417f-9569-0d05ef823c15"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9E1E0CD-117F-4E87-A8F3-B0886CF1B5FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56CE6B3A-81B7-4523-A2F2-344ED760FE09}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5752,28 +5787,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9E1E0CD-117F-4E87-A8F3-B0886CF1B5FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{915DD9A7-7D8D-4B51-8AB7-8EA01404FD44}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="747d6e8b-402a-417f-9569-0d05ef823c15"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>